<commit_message>
continue NB analysis: correlations, diff in CENT_DEG, etc.
</commit_message>
<xml_diff>
--- a/lemmas.xlsx
+++ b/lemmas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quirin/promo/sna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D5848E-E502-C048-AA84-60B673F7040F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B328D75-F80C-EE4C-93E2-13F0F73BE842}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5320" yWindow="5900" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6400" yWindow="24460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="overview" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="232">
   <si>
     <t>LEMMA</t>
   </si>
@@ -708,6 +708,30 @@
   </si>
   <si>
     <t>passive</t>
+  </si>
+  <si>
+    <t>eco-anxiety</t>
+  </si>
+  <si>
+    <t>ecocide</t>
+  </si>
+  <si>
+    <t>flight shame</t>
+  </si>
+  <si>
+    <t>global heating</t>
+  </si>
+  <si>
+    <t>&lt;=2012</t>
+  </si>
+  <si>
+    <t>climate denial</t>
+  </si>
+  <si>
+    <t>climate crisis</t>
+  </si>
+  <si>
+    <t>refugee crisis</t>
   </si>
 </sst>
 </file>
@@ -1178,11 +1202,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:K145"/>
+  <dimension ref="A1:K153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="237" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B129" sqref="B129"/>
+      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B154" sqref="B154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3290,12 +3314,55 @@
         <v>8</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A145" t="s">
         <v>222</v>
       </c>
-      <c r="B145" s="3" t="s">
-        <v>188</v>
+      <c r="C145" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A146" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A147" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A148" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A149" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A150" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A151" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A152" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A153" t="s">
+        <v>231</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cont. proc.: cross-test low-cent-deg lexemes
</commit_message>
<xml_diff>
--- a/lemmas.xlsx
+++ b/lemmas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quirin/promo/sna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B01772-5983-7646-AF1E-623651E94A3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9697F8E7-9BE8-3D46-B2A5-589BB09EB7AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6960" yWindow="24460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="233">
   <si>
     <t>LEMMA</t>
   </si>
@@ -1208,8 +1208,8 @@
   <dimension ref="A1:K153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="237" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C147" sqref="C147"/>
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B149" sqref="B149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3328,6 +3328,9 @@
     <row r="146" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A146" t="s">
         <v>224</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.15">

</xml_diff>